<commit_message>
sites partial, path fixes
</commit_message>
<xml_diff>
--- a/site descriptions.xlsx
+++ b/site descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="6400" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="22120" yWindow="5480" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>AA2Day</t>
   </si>
@@ -220,6 +220,24 @@
   </si>
   <si>
     <t>U. Florida dated interface;  25 simulators available (requires Shockwave plugin), others available by subscription.</t>
+  </si>
+  <si>
+    <t>Ageneral</t>
+  </si>
+  <si>
+    <t>DevlpAnes</t>
+  </si>
+  <si>
+    <t>RCA Training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyword-oriented site divided into a few categories, last updated 11/14. </t>
+  </si>
+  <si>
+    <t>Site dedicated to anesthesia education in limited-resource countries. Hosts numerous pdf handouts, seminars, guidelines and textbook.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robust British anesthesia educational modules for medical students and junior trainees. </t>
   </si>
 </sst>
 </file>
@@ -268,8 +286,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -388,7 +416,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -446,6 +474,11 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -503,6 +536,11 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -832,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1068,54 +1106,78 @@
         <v>66</v>
       </c>
     </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C39" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>